<commit_message>
Add some change in the categorical features
</commit_message>
<xml_diff>
--- a/MVA-LAB11-BANK-INDIA D2 REPORT/Metadata.xlsx
+++ b/MVA-LAB11-BANK-INDIA D2 REPORT/Metadata.xlsx
@@ -5,41 +5,32 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zhengyong Ji\Desktop\MDS\MVA\India-bankk project\MVA-LAB11-BANK-INDIA D2 REPORT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Zhengyong Ji\Documents\GitHub\bank_india\MVA-LAB11-BANK-INDIA D2 REPORT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E0D8A60-88EE-409B-A953-8324D3BEFF5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61F7D848-23EF-4ABC-9510-459FA26DEFD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" xr2:uid="{6AAD3D8C-0EF9-498F-9A83-2DC96F3AAC4C}"/>
+    <workbookView xWindow="32280" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{6AAD3D8C-0EF9-498F-9A83-2DC96F3AAC4C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="MetaData Overview" sheetId="1" r:id="rId1"/>
+    <sheet name="Categorital Resume" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$2:$I$22</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Categorital Resume'!$B$27:$B$83</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'MetaData Overview'!$B$2:$J$22</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="227">
   <si>
     <t>Variable</t>
   </si>
@@ -300,6 +291,426 @@
   </si>
   <si>
     <t>[1, 5000]</t>
+  </si>
+  <si>
+    <t>NAME_FAMILY_STATUS</t>
+  </si>
+  <si>
+    <t>Revolving loans</t>
+  </si>
+  <si>
+    <t>Working</t>
+  </si>
+  <si>
+    <t>Secondary / secondary special</t>
+  </si>
+  <si>
+    <t>Married</t>
+  </si>
+  <si>
+    <t>House / apartment</t>
+  </si>
+  <si>
+    <t>Laborers</t>
+  </si>
+  <si>
+    <t>Self-employed</t>
+  </si>
+  <si>
+    <t>Unaccompanied</t>
+  </si>
+  <si>
+    <t>Cash loans</t>
+  </si>
+  <si>
+    <t>Commercial associate</t>
+  </si>
+  <si>
+    <t>Private service staff</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>State servant</t>
+  </si>
+  <si>
+    <t>Higher education</t>
+  </si>
+  <si>
+    <t>Civil marriage</t>
+  </si>
+  <si>
+    <t>High skill tech staff</t>
+  </si>
+  <si>
+    <t>Transport: type 2</t>
+  </si>
+  <si>
+    <t>Spouse, partner</t>
+  </si>
+  <si>
+    <t>Medicine staff</t>
+  </si>
+  <si>
+    <t>Medicine</t>
+  </si>
+  <si>
+    <t>Family</t>
+  </si>
+  <si>
+    <t>Drivers</t>
+  </si>
+  <si>
+    <t>Industry: type 3</t>
+  </si>
+  <si>
+    <t>Business Entity Type 2</t>
+  </si>
+  <si>
+    <t>Business Entity Type 3</t>
+  </si>
+  <si>
+    <t>Widow</t>
+  </si>
+  <si>
+    <t>Sales staff</t>
+  </si>
+  <si>
+    <t>Other_B</t>
+  </si>
+  <si>
+    <t>Single / not married</t>
+  </si>
+  <si>
+    <t>Accountants</t>
+  </si>
+  <si>
+    <t>Government</t>
+  </si>
+  <si>
+    <t>Separated</t>
+  </si>
+  <si>
+    <t>Managers</t>
+  </si>
+  <si>
+    <t>Transport: type 4</t>
+  </si>
+  <si>
+    <t>With parents</t>
+  </si>
+  <si>
+    <t>Military</t>
+  </si>
+  <si>
+    <t>Pensioner</t>
+  </si>
+  <si>
+    <t>Services</t>
+  </si>
+  <si>
+    <t>Core staff</t>
+  </si>
+  <si>
+    <t>Bank</t>
+  </si>
+  <si>
+    <t>Secretaries</t>
+  </si>
+  <si>
+    <t>School</t>
+  </si>
+  <si>
+    <t>Industry: type 11</t>
+  </si>
+  <si>
+    <t>Cooking staff</t>
+  </si>
+  <si>
+    <t>Trade: type 7</t>
+  </si>
+  <si>
+    <t>Emergency</t>
+  </si>
+  <si>
+    <t>Lower secondary</t>
+  </si>
+  <si>
+    <t>Municipal apartment</t>
+  </si>
+  <si>
+    <t>Industry: type 9</t>
+  </si>
+  <si>
+    <t>Incomplete higher</t>
+  </si>
+  <si>
+    <t>Realty agents</t>
+  </si>
+  <si>
+    <t>Security staff</t>
+  </si>
+  <si>
+    <t>Construction</t>
+  </si>
+  <si>
+    <t>Housing</t>
+  </si>
+  <si>
+    <t>Cleaning staff</t>
+  </si>
+  <si>
+    <t>Business Entity Type 1</t>
+  </si>
+  <si>
+    <t>Rented apartment</t>
+  </si>
+  <si>
+    <t>Mobile</t>
+  </si>
+  <si>
+    <t>Kindergarten</t>
+  </si>
+  <si>
+    <t>Group of people</t>
+  </si>
+  <si>
+    <t>Police</t>
+  </si>
+  <si>
+    <t>Security</t>
+  </si>
+  <si>
+    <t>Postal</t>
+  </si>
+  <si>
+    <t>Agriculture</t>
+  </si>
+  <si>
+    <t>Advertising</t>
+  </si>
+  <si>
+    <t>Low-skill Laborers</t>
+  </si>
+  <si>
+    <t>Industry: type 7</t>
+  </si>
+  <si>
+    <t>Industry: type 1</t>
+  </si>
+  <si>
+    <t>Security Ministries</t>
+  </si>
+  <si>
+    <t>Children</t>
+  </si>
+  <si>
+    <t>Trade: type 3</t>
+  </si>
+  <si>
+    <t>Trade: type 6</t>
+  </si>
+  <si>
+    <t>Hotel</t>
+  </si>
+  <si>
+    <t>Legal Services</t>
+  </si>
+  <si>
+    <t>Trade: type 2</t>
+  </si>
+  <si>
+    <t>Cleaning</t>
+  </si>
+  <si>
+    <t>Trade: type 1</t>
+  </si>
+  <si>
+    <t>Electricity</t>
+  </si>
+  <si>
+    <t>Religion</t>
+  </si>
+  <si>
+    <t>Office apartment</t>
+  </si>
+  <si>
+    <t>HR staff</t>
+  </si>
+  <si>
+    <t>Restaurant</t>
+  </si>
+  <si>
+    <t>Insurance</t>
+  </si>
+  <si>
+    <t>Culture</t>
+  </si>
+  <si>
+    <t>Other_A</t>
+  </si>
+  <si>
+    <t>Telecom</t>
+  </si>
+  <si>
+    <t>Waiters/barmen staff</t>
+  </si>
+  <si>
+    <t>University</t>
+  </si>
+  <si>
+    <t>Academic degree</t>
+  </si>
+  <si>
+    <t>Realtor</t>
+  </si>
+  <si>
+    <t>Co-op apartment</t>
+  </si>
+  <si>
+    <t>IT staff</t>
+  </si>
+  <si>
+    <t>Industry: type 4</t>
+  </si>
+  <si>
+    <t>Industry: type 6</t>
+  </si>
+  <si>
+    <t>Industry: type 12</t>
+  </si>
+  <si>
+    <t>Transport: type 3</t>
+  </si>
+  <si>
+    <t>Transport: type 1</t>
+  </si>
+  <si>
+    <t>Industry: type 2</t>
+  </si>
+  <si>
+    <t>Industry: type 8</t>
+  </si>
+  <si>
+    <t>Industry: type 5</t>
+  </si>
+  <si>
+    <t>Trade: type 4</t>
+  </si>
+  <si>
+    <t>Industry: type 10</t>
+  </si>
+  <si>
+    <t>Categorical Variable</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>target</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>income</t>
+  </si>
+  <si>
+    <t>credit</t>
+  </si>
+  <si>
+    <t>loan</t>
+  </si>
+  <si>
+    <t>family</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>occupation</t>
+  </si>
+  <si>
+    <t>contract</t>
+  </si>
+  <si>
+    <t>car</t>
+  </si>
+  <si>
+    <t>n_child</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>job_stat</t>
+  </si>
+  <si>
+    <t>studies</t>
+  </si>
+  <si>
+    <t>house</t>
+  </si>
+  <si>
+    <t>job_duration</t>
+  </si>
+  <si>
+    <t>job_type</t>
+  </si>
+  <si>
+    <t>n_enquiries</t>
+  </si>
+  <si>
+    <t>companion</t>
+  </si>
+  <si>
+    <t>R name</t>
+  </si>
+  <si>
+    <t>Shorter Categorical Variable</t>
+  </si>
+  <si>
+    <t>Secondary/special</t>
+  </si>
+  <si>
+    <t>Single</t>
+  </si>
+  <si>
+    <t>Divorce</t>
+  </si>
+  <si>
+    <t>Municipal apart.</t>
+  </si>
+  <si>
+    <t>Rented apart</t>
+  </si>
+  <si>
+    <t>Office apart.</t>
+  </si>
+  <si>
+    <t>Co-op apart.</t>
+  </si>
+  <si>
+    <t>House/apartment</t>
+  </si>
+  <si>
+    <t>High-tech staff</t>
+  </si>
+  <si>
+    <t>Medics</t>
+  </si>
+  <si>
+    <t>Chef</t>
+  </si>
+  <si>
+    <t>Waiters staff</t>
+  </si>
+  <si>
+    <t>Organization_type</t>
+  </si>
+  <si>
+    <t>same</t>
   </si>
 </sst>
 </file>
@@ -371,12 +782,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -691,28 +1103,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50D8E44D-ED8D-4963-B656-01C65C739C9F}">
-  <dimension ref="B2:I22"/>
+  <dimension ref="B2:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
     <col min="2" max="2" width="33.1796875" customWidth="1"/>
     <col min="3" max="3" width="29.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="80.1796875" customWidth="1"/>
-    <col min="5" max="5" width="14.08984375" customWidth="1"/>
-    <col min="6" max="6" width="17.1796875" customWidth="1"/>
-    <col min="7" max="7" width="13.36328125" customWidth="1"/>
-    <col min="8" max="8" width="20.1796875" customWidth="1"/>
-    <col min="9" max="9" width="13" customWidth="1"/>
-    <col min="10" max="10" width="14.6328125" customWidth="1"/>
-    <col min="11" max="11" width="7.453125" customWidth="1"/>
-    <col min="12" max="12" width="7.08984375" customWidth="1"/>
+    <col min="4" max="4" width="13.36328125" customWidth="1"/>
+    <col min="5" max="5" width="80.1796875" customWidth="1"/>
+    <col min="6" max="6" width="14.08984375" customWidth="1"/>
+    <col min="7" max="7" width="17.1796875" customWidth="1"/>
+    <col min="8" max="8" width="13.36328125" customWidth="1"/>
+    <col min="9" max="9" width="20.1796875" customWidth="1"/>
+    <col min="10" max="10" width="13" customWidth="1"/>
+    <col min="11" max="11" width="14.6328125" customWidth="1"/>
+    <col min="12" max="12" width="7.453125" customWidth="1"/>
+    <col min="13" max="13" width="7.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9">
+    <row r="2" spans="2:10">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -720,25 +1133,28 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="2:9">
+    <row r="3" spans="2:10">
       <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
@@ -746,21 +1162,24 @@
         <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="2"/>
       <c r="G3" s="2"/>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="2"/>
+      <c r="I3" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="2:9">
+    <row r="4" spans="2:10">
       <c r="B4" s="2" t="s">
         <v>12</v>
       </c>
@@ -768,19 +1187,22 @@
         <v>13</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="2"/>
+      <c r="J4" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="2:9">
+    <row r="5" spans="2:10">
       <c r="B5" s="2" t="s">
         <v>77</v>
       </c>
@@ -788,19 +1210,22 @@
         <v>17</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
-      <c r="I5" s="2" t="s">
+      <c r="I5" s="2"/>
+      <c r="J5" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="2:9">
+    <row r="6" spans="2:10">
       <c r="B6" s="2" t="s">
         <v>73</v>
       </c>
@@ -808,21 +1233,24 @@
         <v>19</v>
       </c>
       <c r="D6" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="2"/>
+      <c r="H6" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2" t="s">
+      <c r="I6" s="2"/>
+      <c r="J6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="2:9">
+    <row r="7" spans="2:10">
       <c r="B7" s="2" t="s">
         <v>74</v>
       </c>
@@ -830,19 +1258,22 @@
         <v>21</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
-      <c r="I7" s="2" t="s">
+      <c r="I7" s="2"/>
+      <c r="J7" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="2:9">
+    <row r="8" spans="2:10">
       <c r="B8" s="2" t="s">
         <v>76</v>
       </c>
@@ -850,23 +1281,26 @@
         <v>22</v>
       </c>
       <c r="D8" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="G8" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2" t="s">
+      <c r="H8" s="2"/>
+      <c r="I8" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="J8" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="2:9">
+    <row r="9" spans="2:10">
       <c r="B9" s="2" t="s">
         <v>75</v>
       </c>
@@ -874,23 +1308,26 @@
         <v>24</v>
       </c>
       <c r="D9" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="F9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="G9" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2" t="s">
+      <c r="H9" s="2"/>
+      <c r="I9" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="J9" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="2:9">
+    <row r="10" spans="2:10">
       <c r="B10" s="2" t="s">
         <v>26</v>
       </c>
@@ -898,23 +1335,26 @@
         <v>27</v>
       </c>
       <c r="D10" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="G10" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2" t="s">
+      <c r="H10" s="2"/>
+      <c r="I10" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="I10" s="2" t="s">
+      <c r="J10" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="2:9">
+    <row r="11" spans="2:10">
       <c r="B11" s="2" t="s">
         <v>30</v>
       </c>
@@ -922,23 +1362,26 @@
         <v>29</v>
       </c>
       <c r="D11" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="F11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="G11" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2" t="s">
+      <c r="H11" s="2"/>
+      <c r="I11" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I11" s="2" t="s">
+      <c r="J11" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="2:9">
+    <row r="12" spans="2:10">
       <c r="B12" s="2" t="s">
         <v>31</v>
       </c>
@@ -946,245 +1389,1381 @@
         <v>32</v>
       </c>
       <c r="D12" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="F12" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="G12" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="H12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="I12" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="I12" s="2" t="s">
+      <c r="J12" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="2:9">
+    <row r="13" spans="2:10">
       <c r="B13" s="2" t="s">
         <v>40</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="F13" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
-      <c r="I13" s="2" t="s">
+      <c r="I13" s="2"/>
+      <c r="J13" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="2:9">
+    <row r="14" spans="2:10">
       <c r="B14" s="2" t="s">
         <v>43</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="E14" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="F14" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
-      <c r="I14" s="2" t="s">
+      <c r="I14" s="2"/>
+      <c r="J14" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="2:9">
+    <row r="15" spans="2:10">
       <c r="B15" s="4" t="s">
         <v>46</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="F15" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
-      <c r="I15" s="2" t="s">
+      <c r="I15" s="2"/>
+      <c r="J15" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="2:9">
+    <row r="16" spans="2:10">
       <c r="B16" s="2" t="s">
         <v>49</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="E16" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="F16" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
-      <c r="I16" s="2" t="s">
+      <c r="I16" s="2"/>
+      <c r="J16" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="2:9">
+    <row r="17" spans="2:10">
       <c r="B17" s="4" t="s">
         <v>52</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="E17" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="F17" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="G17" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2" t="s">
+      <c r="H17" s="2"/>
+      <c r="I17" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="I17" s="2" t="s">
+      <c r="J17" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="2:9">
+    <row r="18" spans="2:10">
       <c r="B18" s="2" t="s">
         <v>56</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="E18" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="F18" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="G18" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2" t="s">
+      <c r="H18" s="2"/>
+      <c r="I18" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="I18" s="2" t="s">
+      <c r="J18" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="2:9">
+    <row r="19" spans="2:10">
       <c r="B19" s="4" t="s">
         <v>78</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="E19" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="F19" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2" t="s">
+      <c r="G19" s="2"/>
+      <c r="H19" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2" t="s">
+      <c r="I19" s="2"/>
+      <c r="J19" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="2:9">
+    <row r="20" spans="2:10">
       <c r="B20" s="2" t="s">
         <v>63</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="E20" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="F20" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
-      <c r="I20" s="2" t="s">
+      <c r="I20" s="2"/>
+      <c r="J20" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="2:9">
+    <row r="21" spans="2:10">
       <c r="B21" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D21" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="E21" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="F21" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F21" s="4" t="s">
+      <c r="G21" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="H21" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H21" s="2" t="s">
+      <c r="I21" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="I21" s="2" t="s">
+      <c r="J21" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="2:9">
+    <row r="22" spans="2:10">
       <c r="B22" s="4" t="s">
         <v>70</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D22" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="E22" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="F22" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2" t="s">
+      <c r="G22" s="2"/>
+      <c r="H22" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2" t="s">
+      <c r="I22" s="2"/>
+      <c r="J22" s="2" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B2:I22" xr:uid="{50D8E44D-ED8D-4963-B656-01C65C739C9F}"/>
+  <autoFilter ref="B2:J22" xr:uid="{50D8E44D-ED8D-4963-B656-01C65C739C9F}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64F8B64E-2CDA-40FF-9288-BEADF5DCD814}">
+  <dimension ref="A1:BE83"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="23.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="26.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.6328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.08984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:57">
+      <c r="A1" s="5" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="2" spans="1:57">
+      <c r="A2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:57">
+      <c r="A3" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:57">
+      <c r="A4" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D4" t="s">
+        <v>134</v>
+      </c>
+      <c r="E4" t="s">
+        <v>137</v>
+      </c>
+      <c r="F4" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="5" spans="1:57">
+      <c r="A5" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" t="s">
+        <v>113</v>
+      </c>
+      <c r="E5" t="s">
+        <v>116</v>
+      </c>
+      <c r="F5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:57">
+      <c r="A6" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" t="s">
+        <v>122</v>
+      </c>
+      <c r="D6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E6" t="s">
+        <v>144</v>
+      </c>
+      <c r="F6" t="s">
+        <v>167</v>
+      </c>
+      <c r="G6" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="7" spans="1:57">
+      <c r="A7" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C7" t="s">
+        <v>98</v>
+      </c>
+      <c r="D7" t="s">
+        <v>103</v>
+      </c>
+      <c r="E7" t="s">
+        <v>106</v>
+      </c>
+      <c r="F7" t="s">
+        <v>109</v>
+      </c>
+      <c r="G7" t="s">
+        <v>114</v>
+      </c>
+      <c r="H7" t="s">
+        <v>117</v>
+      </c>
+      <c r="I7" t="s">
+        <v>120</v>
+      </c>
+      <c r="J7" t="s">
+        <v>126</v>
+      </c>
+      <c r="K7" t="s">
+        <v>128</v>
+      </c>
+      <c r="L7" t="s">
+        <v>131</v>
+      </c>
+      <c r="M7" t="s">
+        <v>138</v>
+      </c>
+      <c r="N7" t="s">
+        <v>139</v>
+      </c>
+      <c r="O7" t="s">
+        <v>142</v>
+      </c>
+      <c r="P7" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>168</v>
+      </c>
+      <c r="R7" t="s">
+        <v>174</v>
+      </c>
+      <c r="S7" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="8" spans="1:57">
+      <c r="A8" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C8" t="s">
+        <v>99</v>
+      </c>
+      <c r="D8" t="s">
+        <v>104</v>
+      </c>
+      <c r="E8" t="s">
+        <v>107</v>
+      </c>
+      <c r="F8" t="s">
+        <v>110</v>
+      </c>
+      <c r="G8" t="s">
+        <v>111</v>
+      </c>
+      <c r="H8" t="s">
+        <v>112</v>
+      </c>
+      <c r="I8" t="s">
+        <v>118</v>
+      </c>
+      <c r="J8" t="s">
+        <v>121</v>
+      </c>
+      <c r="K8" t="s">
+        <v>123</v>
+      </c>
+      <c r="L8" t="s">
+        <v>34</v>
+      </c>
+      <c r="M8" t="s">
+        <v>125</v>
+      </c>
+      <c r="N8" t="s">
+        <v>127</v>
+      </c>
+      <c r="O8" t="s">
+        <v>129</v>
+      </c>
+      <c r="P8" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>132</v>
+      </c>
+      <c r="R8" t="s">
+        <v>133</v>
+      </c>
+      <c r="S8" t="s">
+        <v>136</v>
+      </c>
+      <c r="T8" t="s">
+        <v>140</v>
+      </c>
+      <c r="U8" t="s">
+        <v>141</v>
+      </c>
+      <c r="V8" t="s">
+        <v>143</v>
+      </c>
+      <c r="W8" t="s">
+        <v>145</v>
+      </c>
+      <c r="X8" t="s">
+        <v>146</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>148</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>149</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>150</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>151</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>152</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>154</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>155</v>
+      </c>
+      <c r="AF8" t="s">
+        <v>156</v>
+      </c>
+      <c r="AG8" t="s">
+        <v>158</v>
+      </c>
+      <c r="AH8" t="s">
+        <v>159</v>
+      </c>
+      <c r="AI8" t="s">
+        <v>160</v>
+      </c>
+      <c r="AJ8" t="s">
+        <v>161</v>
+      </c>
+      <c r="AK8" t="s">
+        <v>162</v>
+      </c>
+      <c r="AL8" t="s">
+        <v>163</v>
+      </c>
+      <c r="AM8" t="s">
+        <v>164</v>
+      </c>
+      <c r="AN8" t="s">
+        <v>165</v>
+      </c>
+      <c r="AO8" t="s">
+        <v>166</v>
+      </c>
+      <c r="AP8" t="s">
+        <v>169</v>
+      </c>
+      <c r="AQ8" t="s">
+        <v>170</v>
+      </c>
+      <c r="AR8" t="s">
+        <v>171</v>
+      </c>
+      <c r="AS8" t="s">
+        <v>173</v>
+      </c>
+      <c r="AT8" t="s">
+        <v>175</v>
+      </c>
+      <c r="AU8" t="s">
+        <v>177</v>
+      </c>
+      <c r="AV8" t="s">
+        <v>180</v>
+      </c>
+      <c r="AW8" t="s">
+        <v>181</v>
+      </c>
+      <c r="AX8" t="s">
+        <v>182</v>
+      </c>
+      <c r="AY8" t="s">
+        <v>183</v>
+      </c>
+      <c r="AZ8" t="s">
+        <v>184</v>
+      </c>
+      <c r="BA8" t="s">
+        <v>185</v>
+      </c>
+      <c r="BB8" t="s">
+        <v>186</v>
+      </c>
+      <c r="BC8" t="s">
+        <v>187</v>
+      </c>
+      <c r="BD8" t="s">
+        <v>188</v>
+      </c>
+      <c r="BE8" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="9" spans="1:57">
+      <c r="A9" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" t="s">
+        <v>95</v>
+      </c>
+      <c r="C9" t="s">
+        <v>105</v>
+      </c>
+      <c r="D9" t="s">
+        <v>108</v>
+      </c>
+      <c r="E9" t="s">
+        <v>115</v>
+      </c>
+      <c r="F9" t="s">
+        <v>147</v>
+      </c>
+      <c r="G9" t="s">
+        <v>157</v>
+      </c>
+      <c r="H9" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="14" spans="1:57">
+      <c r="A14" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="15" spans="1:57">
+      <c r="A15" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" t="s">
+        <v>88</v>
+      </c>
+      <c r="C15" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="16" spans="1:57">
+      <c r="A16" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" t="s">
+        <v>89</v>
+      </c>
+      <c r="C16" t="s">
+        <v>97</v>
+      </c>
+      <c r="D16" t="s">
+        <v>100</v>
+      </c>
+      <c r="E16" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="17" spans="1:57">
+      <c r="A17" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" t="s">
+        <v>213</v>
+      </c>
+      <c r="C17" t="s">
+        <v>101</v>
+      </c>
+      <c r="D17" t="s">
+        <v>134</v>
+      </c>
+      <c r="E17" t="s">
+        <v>137</v>
+      </c>
+      <c r="F17" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="18" spans="1:57">
+      <c r="A18" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B18" t="s">
+        <v>91</v>
+      </c>
+      <c r="C18" t="s">
+        <v>102</v>
+      </c>
+      <c r="D18" t="s">
+        <v>113</v>
+      </c>
+      <c r="E18" t="s">
+        <v>214</v>
+      </c>
+      <c r="F18" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="19" spans="1:57">
+      <c r="A19" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" t="s">
+        <v>220</v>
+      </c>
+      <c r="C19" t="s">
+        <v>122</v>
+      </c>
+      <c r="D19" t="s">
+        <v>216</v>
+      </c>
+      <c r="E19" t="s">
+        <v>217</v>
+      </c>
+      <c r="F19" t="s">
+        <v>218</v>
+      </c>
+      <c r="G19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="20" spans="1:57">
+      <c r="A20" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20" t="s">
+        <v>93</v>
+      </c>
+      <c r="C20" t="s">
+        <v>98</v>
+      </c>
+      <c r="D20" t="s">
+        <v>221</v>
+      </c>
+      <c r="E20" t="s">
+        <v>222</v>
+      </c>
+      <c r="F20" t="s">
+        <v>109</v>
+      </c>
+      <c r="G20" t="s">
+        <v>114</v>
+      </c>
+      <c r="H20" t="s">
+        <v>117</v>
+      </c>
+      <c r="I20" t="s">
+        <v>120</v>
+      </c>
+      <c r="J20" t="s">
+        <v>126</v>
+      </c>
+      <c r="K20" t="s">
+        <v>128</v>
+      </c>
+      <c r="L20" t="s">
+        <v>223</v>
+      </c>
+      <c r="M20" t="s">
+        <v>138</v>
+      </c>
+      <c r="N20" t="s">
+        <v>149</v>
+      </c>
+      <c r="O20" t="s">
+        <v>142</v>
+      </c>
+      <c r="P20" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>168</v>
+      </c>
+      <c r="R20" t="s">
+        <v>224</v>
+      </c>
+      <c r="S20" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="21" spans="1:57">
+      <c r="A21" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B21" t="s">
+        <v>94</v>
+      </c>
+      <c r="C21" t="s">
+        <v>99</v>
+      </c>
+      <c r="D21" t="s">
+        <v>104</v>
+      </c>
+      <c r="E21" t="s">
+        <v>107</v>
+      </c>
+      <c r="F21" t="s">
+        <v>110</v>
+      </c>
+      <c r="G21" t="s">
+        <v>111</v>
+      </c>
+      <c r="H21" t="s">
+        <v>112</v>
+      </c>
+      <c r="I21" t="s">
+        <v>118</v>
+      </c>
+      <c r="J21" t="s">
+        <v>121</v>
+      </c>
+      <c r="K21" t="s">
+        <v>123</v>
+      </c>
+      <c r="L21" t="s">
+        <v>34</v>
+      </c>
+      <c r="M21" t="s">
+        <v>125</v>
+      </c>
+      <c r="N21" t="s">
+        <v>127</v>
+      </c>
+      <c r="O21" t="s">
+        <v>129</v>
+      </c>
+      <c r="P21" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>132</v>
+      </c>
+      <c r="R21" t="s">
+        <v>133</v>
+      </c>
+      <c r="S21" t="s">
+        <v>136</v>
+      </c>
+      <c r="T21" t="s">
+        <v>140</v>
+      </c>
+      <c r="U21" t="s">
+        <v>141</v>
+      </c>
+      <c r="V21" t="s">
+        <v>143</v>
+      </c>
+      <c r="W21" t="s">
+        <v>145</v>
+      </c>
+      <c r="X21" t="s">
+        <v>146</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>148</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>149</v>
+      </c>
+      <c r="AA21" t="s">
+        <v>150</v>
+      </c>
+      <c r="AB21" t="s">
+        <v>151</v>
+      </c>
+      <c r="AC21" t="s">
+        <v>152</v>
+      </c>
+      <c r="AD21" t="s">
+        <v>154</v>
+      </c>
+      <c r="AE21" t="s">
+        <v>155</v>
+      </c>
+      <c r="AF21" t="s">
+        <v>156</v>
+      </c>
+      <c r="AG21" t="s">
+        <v>158</v>
+      </c>
+      <c r="AH21" t="s">
+        <v>159</v>
+      </c>
+      <c r="AI21" t="s">
+        <v>160</v>
+      </c>
+      <c r="AJ21" t="s">
+        <v>161</v>
+      </c>
+      <c r="AK21" t="s">
+        <v>162</v>
+      </c>
+      <c r="AL21" t="s">
+        <v>163</v>
+      </c>
+      <c r="AM21" t="s">
+        <v>164</v>
+      </c>
+      <c r="AN21" t="s">
+        <v>165</v>
+      </c>
+      <c r="AO21" t="s">
+        <v>166</v>
+      </c>
+      <c r="AP21" t="s">
+        <v>169</v>
+      </c>
+      <c r="AQ21" t="s">
+        <v>170</v>
+      </c>
+      <c r="AR21" t="s">
+        <v>171</v>
+      </c>
+      <c r="AS21" t="s">
+        <v>173</v>
+      </c>
+      <c r="AT21" t="s">
+        <v>175</v>
+      </c>
+      <c r="AU21" t="s">
+        <v>177</v>
+      </c>
+      <c r="AV21" t="s">
+        <v>180</v>
+      </c>
+      <c r="AW21" t="s">
+        <v>181</v>
+      </c>
+      <c r="AX21" t="s">
+        <v>182</v>
+      </c>
+      <c r="AY21" t="s">
+        <v>183</v>
+      </c>
+      <c r="AZ21" t="s">
+        <v>184</v>
+      </c>
+      <c r="BA21" t="s">
+        <v>185</v>
+      </c>
+      <c r="BB21" t="s">
+        <v>186</v>
+      </c>
+      <c r="BC21" t="s">
+        <v>187</v>
+      </c>
+      <c r="BD21" t="s">
+        <v>188</v>
+      </c>
+      <c r="BE21" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="22" spans="1:57">
+      <c r="A22" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B22" t="s">
+        <v>95</v>
+      </c>
+      <c r="C22" t="s">
+        <v>105</v>
+      </c>
+      <c r="D22" t="s">
+        <v>108</v>
+      </c>
+      <c r="E22" t="s">
+        <v>115</v>
+      </c>
+      <c r="F22" t="s">
+        <v>147</v>
+      </c>
+      <c r="G22" t="s">
+        <v>157</v>
+      </c>
+      <c r="H22" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="27" spans="1:57">
+      <c r="B27" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="28" spans="1:57">
+      <c r="B28" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="29" spans="1:57">
+      <c r="B29" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="30" spans="1:57">
+      <c r="B30" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="31" spans="1:57">
+      <c r="B31" t="s">
+        <v>143</v>
+      </c>
+      <c r="C31" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="32" spans="1:57">
+      <c r="B32" t="s">
+        <v>111</v>
+      </c>
+      <c r="C32" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3">
+      <c r="B33" t="s">
+        <v>112</v>
+      </c>
+      <c r="C33" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3">
+      <c r="B34" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3">
+      <c r="B35" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3">
+      <c r="B36" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3">
+      <c r="B37" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3">
+      <c r="B38" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3">
+      <c r="B39" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3">
+      <c r="B40" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3">
+      <c r="B41" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3">
+      <c r="B42" t="s">
+        <v>155</v>
+      </c>
+      <c r="C42" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3">
+      <c r="B43" t="s">
+        <v>189</v>
+      </c>
+      <c r="C43" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3">
+      <c r="B44" t="s">
+        <v>130</v>
+      </c>
+      <c r="C44" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3">
+      <c r="B45" t="s">
+        <v>182</v>
+      </c>
+      <c r="C45" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3">
+      <c r="B46" t="s">
+        <v>185</v>
+      </c>
+      <c r="C46" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3">
+      <c r="B47" t="s">
+        <v>110</v>
+      </c>
+      <c r="C47" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3">
+      <c r="B48" t="s">
+        <v>180</v>
+      </c>
+      <c r="C48" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3">
+      <c r="B49" t="s">
+        <v>187</v>
+      </c>
+      <c r="C49" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3">
+      <c r="B50" t="s">
+        <v>181</v>
+      </c>
+      <c r="C50" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3">
+      <c r="B51" t="s">
+        <v>154</v>
+      </c>
+      <c r="C51" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3">
+      <c r="B52" t="s">
+        <v>186</v>
+      </c>
+      <c r="C52" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3">
+      <c r="B53" t="s">
+        <v>136</v>
+      </c>
+      <c r="C53" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3">
+      <c r="B54" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3">
+      <c r="B55" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3">
+      <c r="B56" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3">
+      <c r="B57" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3">
+      <c r="B58" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3">
+      <c r="B59" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3">
+      <c r="B60" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3">
+      <c r="B61" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3">
+      <c r="B62" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="63" spans="2:3">
+      <c r="B63" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="64" spans="2:3">
+      <c r="B64" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3">
+      <c r="B65" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3">
+      <c r="B66" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="67" spans="2:3">
+      <c r="B67" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="68" spans="2:3">
+      <c r="B68" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3">
+      <c r="B69" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="70" spans="2:3">
+      <c r="B70" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="71" spans="2:3">
+      <c r="B71" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="72" spans="2:3">
+      <c r="B72" t="s">
+        <v>164</v>
+      </c>
+      <c r="C72" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="73" spans="2:3">
+      <c r="B73" t="s">
+        <v>162</v>
+      </c>
+      <c r="C73" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="74" spans="2:3">
+      <c r="B74" t="s">
+        <v>158</v>
+      </c>
+      <c r="C74" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="75" spans="2:3">
+      <c r="B75" t="s">
+        <v>188</v>
+      </c>
+      <c r="C75" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="76" spans="2:3">
+      <c r="B76" t="s">
+        <v>159</v>
+      </c>
+      <c r="C76" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="77" spans="2:3">
+      <c r="B77" t="s">
+        <v>132</v>
+      </c>
+      <c r="C77" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="78" spans="2:3">
+      <c r="B78" t="s">
+        <v>184</v>
+      </c>
+      <c r="C78" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="79" spans="2:3">
+      <c r="B79" t="s">
+        <v>104</v>
+      </c>
+      <c r="C79" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="80" spans="2:3">
+      <c r="B80" t="s">
+        <v>183</v>
+      </c>
+      <c r="C80" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="81" spans="2:3">
+      <c r="B81" t="s">
+        <v>121</v>
+      </c>
+      <c r="C81" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="82" spans="2:3">
+      <c r="B82" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="83" spans="2:3">
+      <c r="B83" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="B27:B83" xr:uid="{64F8B64E-2CDA-40FF-9288-BEADF5DCD814}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B28:B83">
+      <sortCondition ref="B27:B83"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Rename Categorical variable and checking possibility to collapse organization type into a smaller one
</commit_message>
<xml_diff>
--- a/MVA-LAB11-BANK-INDIA D2 REPORT/Metadata.xlsx
+++ b/MVA-LAB11-BANK-INDIA D2 REPORT/Metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Zhengyong Ji\Documents\GitHub\bank_india\MVA-LAB11-BANK-INDIA D2 REPORT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61F7D848-23EF-4ABC-9510-459FA26DEFD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E80D8B15-A2C1-49AB-8EC0-6A6E774BCB61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32280" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{6AAD3D8C-0EF9-498F-9A83-2DC96F3AAC4C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" activeTab="1" xr2:uid="{6AAD3D8C-0EF9-498F-9A83-2DC96F3AAC4C}"/>
   </bookViews>
   <sheets>
     <sheet name="MetaData Overview" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="228">
   <si>
     <t>Variable</t>
   </si>
@@ -683,9 +683,6 @@
     <t>Municipal apart.</t>
   </si>
   <si>
-    <t>Rented apart</t>
-  </si>
-  <si>
     <t>Office apart.</t>
   </si>
   <si>
@@ -711,6 +708,12 @@
   </si>
   <si>
     <t>same</t>
+  </si>
+  <si>
+    <t>Partner</t>
+  </si>
+  <si>
+    <t>Rented apart.</t>
   </si>
 </sst>
 </file>
@@ -793,7 +796,18 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1669,8 +1683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64F8B64E-2CDA-40FF-9288-BEADF5DCD814}">
   <dimension ref="A1:BE83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
@@ -2122,7 +2136,7 @@
         <v>50</v>
       </c>
       <c r="B19" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C19" t="s">
         <v>122</v>
@@ -2131,13 +2145,13 @@
         <v>216</v>
       </c>
       <c r="E19" t="s">
+        <v>227</v>
+      </c>
+      <c r="F19" t="s">
         <v>217</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>218</v>
-      </c>
-      <c r="G19" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="20" spans="1:57">
@@ -2151,10 +2165,10 @@
         <v>98</v>
       </c>
       <c r="D20" t="s">
+        <v>220</v>
+      </c>
+      <c r="E20" t="s">
         <v>221</v>
-      </c>
-      <c r="E20" t="s">
-        <v>222</v>
       </c>
       <c r="F20" t="s">
         <v>109</v>
@@ -2175,7 +2189,7 @@
         <v>128</v>
       </c>
       <c r="L20" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="M20" t="s">
         <v>138</v>
@@ -2193,7 +2207,7 @@
         <v>168</v>
       </c>
       <c r="R20" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="S20" t="s">
         <v>179</v>
@@ -2380,7 +2394,7 @@
         <v>95</v>
       </c>
       <c r="C22" t="s">
-        <v>105</v>
+        <v>226</v>
       </c>
       <c r="D22" t="s">
         <v>108</v>
@@ -2400,7 +2414,7 @@
     </row>
     <row r="27" spans="1:57">
       <c r="B27" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="28" spans="1:57">
@@ -2423,7 +2437,7 @@
         <v>143</v>
       </c>
       <c r="C31" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="32" spans="1:57">
@@ -2431,7 +2445,7 @@
         <v>111</v>
       </c>
       <c r="C32" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="33" spans="2:3">
@@ -2439,7 +2453,7 @@
         <v>112</v>
       </c>
       <c r="C33" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="34" spans="2:3">
@@ -2487,7 +2501,7 @@
         <v>155</v>
       </c>
       <c r="C42" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="43" spans="2:3">
@@ -2495,7 +2509,7 @@
         <v>189</v>
       </c>
       <c r="C43" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="44" spans="2:3">
@@ -2503,7 +2517,7 @@
         <v>130</v>
       </c>
       <c r="C44" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="45" spans="2:3">
@@ -2511,7 +2525,7 @@
         <v>182</v>
       </c>
       <c r="C45" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="46" spans="2:3">
@@ -2519,7 +2533,7 @@
         <v>185</v>
       </c>
       <c r="C46" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="47" spans="2:3">
@@ -2527,7 +2541,7 @@
         <v>110</v>
       </c>
       <c r="C47" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="48" spans="2:3">
@@ -2535,7 +2549,7 @@
         <v>180</v>
       </c>
       <c r="C48" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="49" spans="2:3">
@@ -2543,7 +2557,7 @@
         <v>187</v>
       </c>
       <c r="C49" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="50" spans="2:3">
@@ -2551,7 +2565,7 @@
         <v>181</v>
       </c>
       <c r="C50" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="51" spans="2:3">
@@ -2559,7 +2573,7 @@
         <v>154</v>
       </c>
       <c r="C51" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="52" spans="2:3">
@@ -2567,7 +2581,7 @@
         <v>186</v>
       </c>
       <c r="C52" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="53" spans="2:3">
@@ -2575,7 +2589,7 @@
         <v>136</v>
       </c>
       <c r="C53" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="54" spans="2:3">
@@ -2673,7 +2687,7 @@
         <v>164</v>
       </c>
       <c r="C72" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="73" spans="2:3">
@@ -2681,7 +2695,7 @@
         <v>162</v>
       </c>
       <c r="C73" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="74" spans="2:3">
@@ -2689,7 +2703,7 @@
         <v>158</v>
       </c>
       <c r="C74" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="75" spans="2:3">
@@ -2697,7 +2711,7 @@
         <v>188</v>
       </c>
       <c r="C75" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="76" spans="2:3">
@@ -2705,7 +2719,7 @@
         <v>159</v>
       </c>
       <c r="C76" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="77" spans="2:3">
@@ -2713,7 +2727,7 @@
         <v>132</v>
       </c>
       <c r="C77" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="78" spans="2:3">
@@ -2721,7 +2735,7 @@
         <v>184</v>
       </c>
       <c r="C78" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="79" spans="2:3">
@@ -2729,7 +2743,7 @@
         <v>104</v>
       </c>
       <c r="C79" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="80" spans="2:3">
@@ -2737,7 +2751,7 @@
         <v>183</v>
       </c>
       <c r="C80" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="81" spans="2:3">
@@ -2745,7 +2759,7 @@
         <v>121</v>
       </c>
       <c r="C81" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="82" spans="2:3">
@@ -2764,6 +2778,9 @@
       <sortCondition ref="B27:B83"/>
     </sortState>
   </autoFilter>
+  <conditionalFormatting sqref="A1:XFD9 A15:XFD22">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding the Mahalanobis distance for outlier detection
</commit_message>
<xml_diff>
--- a/MVA-LAB11-BANK-INDIA D2 REPORT/Metadata.xlsx
+++ b/MVA-LAB11-BANK-INDIA D2 REPORT/Metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Zhengyong Ji\Documents\GitHub\bank_india\MVA-LAB11-BANK-INDIA D2 REPORT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D215893B-7F98-4AF4-960D-83FE652E7811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38D082EA-9668-4B61-80FF-0BF33F0B8146}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" activeTab="1" xr2:uid="{6AAD3D8C-0EF9-498F-9A83-2DC96F3AAC4C}"/>
+    <workbookView xWindow="32280" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{6AAD3D8C-0EF9-498F-9A83-2DC96F3AAC4C}"/>
   </bookViews>
   <sheets>
     <sheet name="MetaData Overview" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="234">
   <si>
     <t>Variable</t>
   </si>
@@ -698,9 +698,6 @@
     <t>Chef</t>
   </si>
   <si>
-    <t>Waiters staff</t>
-  </si>
-  <si>
     <t>Organization_type</t>
   </si>
   <si>
@@ -729,6 +726,12 @@
   </si>
   <si>
     <t>Group_people</t>
+  </si>
+  <si>
+    <t>Waiters</t>
+  </si>
+  <si>
+    <t>Private serv.</t>
   </si>
 </sst>
 </file>
@@ -1134,8 +1137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50D8E44D-ED8D-4963-B656-01C65C739C9F}">
   <dimension ref="B2:J22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
@@ -1143,7 +1146,7 @@
     <col min="2" max="2" width="33.1796875" customWidth="1"/>
     <col min="3" max="3" width="29.7265625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.36328125" customWidth="1"/>
-    <col min="5" max="5" width="80.1796875" customWidth="1"/>
+    <col min="5" max="5" width="156.26953125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.08984375" customWidth="1"/>
     <col min="7" max="7" width="17.1796875" customWidth="1"/>
     <col min="8" max="8" width="13.36328125" customWidth="1"/>
@@ -1698,8 +1701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64F8B64E-2CDA-40FF-9288-BEADF5DCD814}">
   <dimension ref="A1:BE83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
@@ -2097,7 +2100,7 @@
         <v>89</v>
       </c>
       <c r="C16" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D16" t="s">
         <v>100</v>
@@ -2111,10 +2114,10 @@
         <v>44</v>
       </c>
       <c r="B17" t="s">
+        <v>227</v>
+      </c>
+      <c r="C17" t="s">
         <v>228</v>
-      </c>
-      <c r="C17" t="s">
-        <v>229</v>
       </c>
       <c r="D17" t="s">
         <v>134</v>
@@ -2160,7 +2163,7 @@
         <v>215</v>
       </c>
       <c r="E19" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F19" t="s">
         <v>216</v>
@@ -2177,7 +2180,7 @@
         <v>93</v>
       </c>
       <c r="C20" t="s">
-        <v>98</v>
+        <v>233</v>
       </c>
       <c r="D20" t="s">
         <v>219</v>
@@ -2216,13 +2219,13 @@
         <v>142</v>
       </c>
       <c r="P20" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="Q20" t="s">
         <v>168</v>
       </c>
       <c r="R20" t="s">
-        <v>222</v>
+        <v>232</v>
       </c>
       <c r="S20" t="s">
         <v>179</v>
@@ -2406,10 +2409,10 @@
         <v>71</v>
       </c>
       <c r="B22" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C22" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D22" t="s">
         <v>108</v>
@@ -2418,7 +2421,7 @@
         <v>115</v>
       </c>
       <c r="F22" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G22" t="s">
         <v>157</v>
@@ -2429,7 +2432,7 @@
     </row>
     <row r="27" spans="1:57">
       <c r="B27" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="28" spans="1:57">
@@ -2452,7 +2455,7 @@
         <v>143</v>
       </c>
       <c r="C31" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="32" spans="1:57">
@@ -2460,7 +2463,7 @@
         <v>111</v>
       </c>
       <c r="C32" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="33" spans="2:3">
@@ -2468,7 +2471,7 @@
         <v>112</v>
       </c>
       <c r="C33" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="34" spans="2:3">
@@ -2516,7 +2519,7 @@
         <v>155</v>
       </c>
       <c r="C42" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="43" spans="2:3">
@@ -2524,7 +2527,7 @@
         <v>189</v>
       </c>
       <c r="C43" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="44" spans="2:3">
@@ -2532,7 +2535,7 @@
         <v>130</v>
       </c>
       <c r="C44" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="45" spans="2:3">
@@ -2540,7 +2543,7 @@
         <v>182</v>
       </c>
       <c r="C45" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="46" spans="2:3">
@@ -2548,7 +2551,7 @@
         <v>185</v>
       </c>
       <c r="C46" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="47" spans="2:3">
@@ -2556,7 +2559,7 @@
         <v>110</v>
       </c>
       <c r="C47" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="48" spans="2:3">
@@ -2564,7 +2567,7 @@
         <v>180</v>
       </c>
       <c r="C48" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="49" spans="2:3">
@@ -2572,7 +2575,7 @@
         <v>187</v>
       </c>
       <c r="C49" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="50" spans="2:3">
@@ -2580,7 +2583,7 @@
         <v>181</v>
       </c>
       <c r="C50" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="51" spans="2:3">
@@ -2588,7 +2591,7 @@
         <v>154</v>
       </c>
       <c r="C51" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="52" spans="2:3">
@@ -2596,7 +2599,7 @@
         <v>186</v>
       </c>
       <c r="C52" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="53" spans="2:3">
@@ -2604,7 +2607,7 @@
         <v>136</v>
       </c>
       <c r="C53" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="54" spans="2:3">
@@ -2702,7 +2705,7 @@
         <v>164</v>
       </c>
       <c r="C72" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="73" spans="2:3">
@@ -2710,7 +2713,7 @@
         <v>162</v>
       </c>
       <c r="C73" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="74" spans="2:3">
@@ -2718,7 +2721,7 @@
         <v>158</v>
       </c>
       <c r="C74" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="75" spans="2:3">
@@ -2726,7 +2729,7 @@
         <v>188</v>
       </c>
       <c r="C75" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="76" spans="2:3">
@@ -2734,7 +2737,7 @@
         <v>159</v>
       </c>
       <c r="C76" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="77" spans="2:3">
@@ -2742,7 +2745,7 @@
         <v>132</v>
       </c>
       <c r="C77" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="78" spans="2:3">
@@ -2750,7 +2753,7 @@
         <v>184</v>
       </c>
       <c r="C78" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="79" spans="2:3">
@@ -2758,7 +2761,7 @@
         <v>104</v>
       </c>
       <c r="C79" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="80" spans="2:3">
@@ -2766,7 +2769,7 @@
         <v>183</v>
       </c>
       <c r="C80" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="81" spans="2:3">
@@ -2774,7 +2777,7 @@
         <v>121</v>
       </c>
       <c r="C81" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="82" spans="2:3">

</xml_diff>